<commit_message>
pask samma format som jul, nytt art. nr. semla,
</commit_message>
<xml_diff>
--- a/templates/placeringsnycklar_pask.xlsx
+++ b/templates/placeringsnycklar_pask.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecilia Winkler\Jupyter\WebShopReport\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecilia Winkler\Jupyter\WebShopReport\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAF2AD2-D936-427B-9C55-100181661E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF982D3-B6D3-4474-8B5C-41C4A702A3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kategorier pask" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Kategorier pask'!$A$2:$F$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Kategorier pask'!$A$2:$F$53</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
   <si>
     <t>Område</t>
   </si>
@@ -266,12 +266,6 @@
   </si>
   <si>
     <t>hårdost!</t>
-  </si>
-  <si>
-    <t>Julpynt</t>
-  </si>
-  <si>
-    <t>Pynt</t>
   </si>
   <si>
     <t>Sverige</t>
@@ -945,9 +939,11 @@
   <sheetPr>
     <tabColor rgb="FF99CC00"/>
   </sheetPr>
-  <dimension ref="A2:AMJ54"/>
+  <dimension ref="A2:AMJ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
@@ -1798,7 +1794,7 @@
       </c>
       <c r="B50" s="17" t="str">
         <f>C50&amp;" / "&amp;D50</f>
-        <v>Pynt / Julpynt</v>
+        <v>1-Sv / Sverige</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>75</v>
@@ -1808,7 +1804,6 @@
       </c>
       <c r="F50" s="22"/>
       <c r="I50" s="18"/>
-      <c r="K50" s="23"/>
     </row>
     <row r="51" spans="1:11" s="17" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="17" t="s">
@@ -1816,7 +1811,7 @@
       </c>
       <c r="B51" s="17" t="str">
         <f>C51&amp;" / "&amp;D51</f>
-        <v>1-Sv / Sverige</v>
+        <v>3-Txt / Textil</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>77</v>
@@ -1825,7 +1820,6 @@
         <v>76</v>
       </c>
       <c r="F51" s="22"/>
-      <c r="I51" s="18"/>
     </row>
     <row r="52" spans="1:11" s="17" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="17" t="s">
@@ -1833,7 +1827,7 @@
       </c>
       <c r="B52" s="17" t="str">
         <f>C52&amp;" / "&amp;D52</f>
-        <v>3-Txt / Textil</v>
+        <v>2-Bk / Böcker</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>79</v>
@@ -1843,24 +1837,8 @@
       </c>
       <c r="F52" s="22"/>
     </row>
-    <row r="53" spans="1:11" s="17" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A53" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="17" t="str">
-        <f>C53&amp;" / "&amp;D53</f>
-        <v>2-Bk / Böcker</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F53" s="22"/>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="F54" s="19"/>
+    <row r="53" spans="1:11">
+      <c r="F53" s="19"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>